<commit_message>
Fiddled around with different player ranking methods
</commit_message>
<xml_diff>
--- a/data/2015 Spring Season.xlsx
+++ b/data/2015 Spring Season.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9450"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9450" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Races" sheetId="46" r:id="rId1"/>
@@ -1121,9 +1121,6 @@
     <t>Kyle McKenney</t>
   </si>
   <si>
-    <t>Aleksandr Staprans</t>
-  </si>
-  <si>
     <t>Jonathan Dawson</t>
   </si>
   <si>
@@ -1299,6 +1296,9 @@
   </si>
   <si>
     <t>Aidan Daly-Jensen</t>
+  </si>
+  <si>
+    <t>Aleks Staprans</t>
   </si>
 </sst>
 </file>
@@ -1634,7 +1634,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
@@ -6698,16 +6698,16 @@
         <v>76</v>
       </c>
       <c r="C11" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D11" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E11" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G11" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -6715,16 +6715,16 @@
         <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D12" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E12" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="G12" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -6732,16 +6732,16 @@
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D13" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E13" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="G13" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -6749,16 +6749,16 @@
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D14" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E14" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="G14" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -6766,16 +6766,16 @@
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D15" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="E15" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="G15" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -6783,16 +6783,16 @@
         <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D16" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E16" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="G16" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
@@ -6800,16 +6800,16 @@
         <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D17" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="E17" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="G17" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
@@ -6817,16 +6817,16 @@
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D18" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="E18" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="G18" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
@@ -6834,16 +6834,16 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D19" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="E19" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="G19" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
@@ -8427,8 +8427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8682,10 +8682,10 @@
         <v>85</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>85</v>
@@ -10622,19 +10622,19 @@
         <v>76</v>
       </c>
       <c r="C11" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D11" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="F11" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="G11" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="H11" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -10642,19 +10642,19 @@
         <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D12" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F12" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="G12" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="H12" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -10662,19 +10662,19 @@
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D13" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="F13" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="G13" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="H13" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -10682,19 +10682,19 @@
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D14" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F14" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="G14" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="H14" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -10702,19 +10702,19 @@
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D15" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F15" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="G15" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="H15" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -10722,19 +10722,19 @@
         <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D16" t="s">
+        <v>411</v>
+      </c>
+      <c r="F16" t="s">
         <v>412</v>
       </c>
-      <c r="F16" t="s">
-        <v>413</v>
-      </c>
       <c r="G16" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="H16" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
@@ -10742,19 +10742,19 @@
         <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D17" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="F17" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="G17" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="H17" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
@@ -10762,19 +10762,19 @@
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D18" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="F18" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="G18" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="H18" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
@@ -10782,19 +10782,19 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D19" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="F19" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="G19" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="H19" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
@@ -11057,7 +11057,7 @@
   <dimension ref="A1:P69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11341,10 +11341,10 @@
         <v>353</v>
       </c>
       <c r="G12" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="J12" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
@@ -11358,7 +11358,7 @@
         <v>354</v>
       </c>
       <c r="E13" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F13" t="s">
         <v>356</v>
@@ -11384,13 +11384,13 @@
         <v>355</v>
       </c>
       <c r="F14" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G14" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J14" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
@@ -11404,16 +11404,16 @@
         <v>356</v>
       </c>
       <c r="E15" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F15" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="G15" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="J15" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
@@ -11421,13 +11421,13 @@
         <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>357</v>
+        <v>416</v>
       </c>
       <c r="D16" t="s">
-        <v>357</v>
+        <v>416</v>
       </c>
       <c r="E16" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F16" t="s">
         <v>355</v>
@@ -11444,10 +11444,10 @@
         <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D17" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E17" t="s">
         <v>354</v>
@@ -11456,10 +11456,10 @@
         <v>354</v>
       </c>
       <c r="G17" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="J17" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
@@ -11467,22 +11467,22 @@
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D18" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E18" t="s">
         <v>356</v>
       </c>
       <c r="F18" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G18" t="s">
-        <v>357</v>
+        <v>416</v>
       </c>
       <c r="J18" t="s">
-        <v>357</v>
+        <v>416</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
@@ -11490,22 +11490,22 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D19" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E19" t="s">
+        <v>416</v>
+      </c>
+      <c r="F19" t="s">
+        <v>416</v>
+      </c>
+      <c r="G19" t="s">
         <v>357</v>
       </c>
-      <c r="F19" t="s">
-        <v>357</v>
-      </c>
-      <c r="G19" t="s">
-        <v>358</v>
-      </c>
       <c r="J19" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
@@ -11972,22 +11972,22 @@
         <v>76</v>
       </c>
       <c r="C11" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D11" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E11" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F11" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="G11" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="I11" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -11995,22 +11995,22 @@
         <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D12" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E12" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F12" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="G12" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="I12" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -12018,22 +12018,22 @@
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D13" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E13" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F13" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G13" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="I13" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -12041,22 +12041,22 @@
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D14" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E14" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F14" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G14" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="I14" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -12064,22 +12064,22 @@
         <v>5</v>
       </c>
       <c r="C15" t="s">
+        <v>368</v>
+      </c>
+      <c r="D15" t="s">
         <v>369</v>
       </c>
-      <c r="D15" t="s">
-        <v>370</v>
-      </c>
       <c r="E15" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F15" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G15" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="I15" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -12087,22 +12087,22 @@
         <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D16" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E16" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F16" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="G16" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="I16" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
@@ -12110,22 +12110,22 @@
         <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D17" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E17" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F17" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="G17" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="I17" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
@@ -12133,22 +12133,22 @@
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D18" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E18" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="F18" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="G18" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="I18" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
@@ -12156,22 +12156,22 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D19" t="s">
+        <v>373</v>
+      </c>
+      <c r="E19" t="s">
+        <v>373</v>
+      </c>
+      <c r="F19" t="s">
         <v>374</v>
       </c>
-      <c r="E19" t="s">
+      <c r="G19" t="s">
         <v>374</v>
       </c>
-      <c r="F19" t="s">
-        <v>375</v>
-      </c>
-      <c r="G19" t="s">
-        <v>375</v>
-      </c>
       <c r="I19" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
@@ -12601,10 +12601,10 @@
         <v>76</v>
       </c>
       <c r="C11" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D11" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -12612,10 +12612,10 @@
         <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D12" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -12623,10 +12623,10 @@
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D13" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -12634,10 +12634,10 @@
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D14" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -12645,10 +12645,10 @@
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D15" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -12656,10 +12656,10 @@
         <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D16" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
@@ -12667,10 +12667,10 @@
         <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D17" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
@@ -12678,10 +12678,10 @@
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D18" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
@@ -12689,10 +12689,10 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D19" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
@@ -13115,7 +13115,7 @@
         <v>76</v>
       </c>
       <c r="C11" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -13123,7 +13123,7 @@
         <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -13131,7 +13131,7 @@
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -13139,7 +13139,7 @@
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -13147,7 +13147,7 @@
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -13155,7 +13155,7 @@
         <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
@@ -13163,7 +13163,7 @@
         <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
@@ -13171,7 +13171,7 @@
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
@@ -13179,7 +13179,7 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
@@ -15171,22 +15171,22 @@
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D15" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E15" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="F15" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="H15" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="I15" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fixed some name errors in season
</commit_message>
<xml_diff>
--- a/data/2015 Spring Season.xlsx
+++ b/data/2015 Spring Season.xlsx
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1924" uniqueCount="416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1924" uniqueCount="415">
   <si>
     <t>Jon Bachmann</t>
   </si>
@@ -1287,9 +1287,6 @@
   </si>
   <si>
     <t>Ryan Mallgrave</t>
-  </si>
-  <si>
-    <t>Gugliemo Carcano</t>
   </si>
   <si>
     <t>Aidan Daly-Jensen</t>
@@ -8425,7 +8422,7 @@
   <dimension ref="A1:I69"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8679,10 +8676,10 @@
         <v>85</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>413</v>
+        <v>85</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>413</v>
+        <v>85</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>85</v>
@@ -11418,10 +11415,10 @@
         <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D16" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E16" t="s">
         <v>357</v>
@@ -11476,10 +11473,10 @@
         <v>356</v>
       </c>
       <c r="G18" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="J18" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
@@ -11493,10 +11490,10 @@
         <v>358</v>
       </c>
       <c r="E19" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="F19" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="G19" t="s">
         <v>356</v>
@@ -15168,22 +15165,22 @@
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D15" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E15" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F15" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="H15" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="I15" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>